<commit_message>
update posfront recheck item, deposit, double screen
</commit_message>
<xml_diff>
--- a/madju-credit.xlsx
+++ b/madju-credit.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
     <sheet name="Report" sheetId="10" r:id="rId10"/>
     <sheet name="reportphp" sheetId="11" r:id="rId11"/>
+    <sheet name="barcode" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">API!$A$1:$O$52</definedName>
@@ -109,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6569" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6580" uniqueCount="1134">
   <si>
     <t>No</t>
   </si>
@@ -3423,9 +3424,6 @@
     <t xml:space="preserve">$str="insert into tx_stock_opname(itemcode,itemname,warehouse,qty,unit,createdate,updatedate) values('$dt[1]','$dt[2]','$dt[3]','$dt[11]','$dt[6]',now(),now())";include("exec2.php"); </t>
   </si>
   <si>
-    <t>SUM(a.beginqty+a.inqty+a.outqty-a.opnameqty)</t>
-  </si>
-  <si>
     <t>SUM(a.beginqty)</t>
   </si>
   <si>
@@ -3435,18 +3433,9 @@
     <t>SUM(a.outqty)</t>
   </si>
   <si>
-    <t>SUM(a.beginqty+a.inqty+a.outqty)</t>
-  </si>
-  <si>
     <t>SUM(a.opnameqty)</t>
   </si>
   <si>
-    <t>; from tx_stock_all a where a.itemcode&lt;&gt;"" GROUP BY a.itemname,a.warehouse,IFNULL(a.unit,"") order by itemname ;</t>
-  </si>
-  <si>
-    <t>; from tx_stock_all a where   a.itemcode&lt;&gt;"" and concat(itemname) like "%w2%"  GROUP BY a.itemname,a.warehouse,IFNULL(a.unit,"")  order by itemname ;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> $i=0;$dt1=explode('{}', $dt[19]);$str="INSERT INTO tx_stock_all(itemcode,itemname,unit,userid,transtime,transdesc,warehouse,outqty) values"; if ($dt1!='') {   foreach($dt1 as $loop)    {$dt2 = explode('[]',$dt1[$i]); $str=$str."('$dt2[2]','$dt2[3]','$dt2[5]','$user',now(),'Sales Credit #$dt2[0]','$dt[5]',$dt2[4]),";  $i++; }$str=substr($str, 0, -1);include("exec2.php"); }</t>
   </si>
   <si>
@@ -3508,13 +3497,58 @@
   </si>
   <si>
     <t>"delete from tx_stock_opname where itemcode='$dt[0]' and and warehouse='$dt[2]'";</t>
+  </si>
+  <si>
+    <t>; from tx_stock_all a where   a.itemcode&lt;&gt;"" and transtime&gt;=(select description from ms_setting where settingtype="opnamestart")  and concat(itemname) like "%w2%"  GROUP BY a.itemname,a.warehouse,IFNULL(a.unit,"")  order by itemname ;</t>
+  </si>
+  <si>
+    <t>; from tx_stock_all a where a.itemcode&lt;&gt;"" and transtime&gt;=(select description from ms_setting where settingtype="opnamestart") GROUP BY a.itemname,a.warehouse,IFNULL(a.unit,"") order by itemname ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$str="insert into tx_stock_all(itemcode,itemname,userid,transtime,transdesc,warehouse,inqty,outqty,beginqty,opnameqty,unit) values('$dt[1]','$dt[2]','$user',now(),'Begin Stock','$dt[3]',0,0,'$dt[4]',0,'$dt[5]')";include("exec2.php"); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUM(a.beginqty)+SUM(a.inqty)-SUM(a.outqty) </t>
+  </si>
+  <si>
+    <t>SUM(a.beginqty)+SUM(a.inqty)-SUM(a.outqty) -sum(a.opnameqty)</t>
+  </si>
+  <si>
+    <t>*8001*</t>
+  </si>
+  <si>
+    <t>*8002*</t>
+  </si>
+  <si>
+    <t>*8003*</t>
+  </si>
+  <si>
+    <t>*8004*</t>
+  </si>
+  <si>
+    <t>*8005*</t>
+  </si>
+  <si>
+    <t>*9001*</t>
+  </si>
+  <si>
+    <t>*9002*</t>
+  </si>
+  <si>
+    <t>*9003*</t>
+  </si>
+  <si>
+    <t>*9004*</t>
+  </si>
+  <si>
+    <t>*9005*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3536,6 +3570,20 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Free 3 of 9"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3588,7 +3636,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
@@ -3652,6 +3700,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3949,6 +4002,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
@@ -4401,6 +4455,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4713,6 +4768,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4851,8 +4907,122 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet12"/>
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="48"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" style="30" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="31" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A1" s="29" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+    </row>
+    <row r="2" spans="1:4" ht="41.25">
+      <c r="A2" s="29" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+    </row>
+    <row r="3" spans="1:4" ht="41.25">
+      <c r="A3" s="29" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+    </row>
+    <row r="4" spans="1:4" ht="41.25">
+      <c r="A4" s="29" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+    </row>
+    <row r="5" spans="1:4" ht="41.25">
+      <c r="A5" s="29" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+    </row>
+    <row r="6" spans="1:4" ht="41.25">
+      <c r="A6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+    </row>
+    <row r="7" spans="1:4" ht="41.25">
+      <c r="A7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+    </row>
+    <row r="8" spans="1:4" ht="41.25">
+      <c r="A8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+    </row>
+    <row r="9" spans="1:4" ht="41.25">
+      <c r="A9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+    </row>
+    <row r="10" spans="1:4" ht="41.25">
+      <c r="A10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+    </row>
+    <row r="11" spans="1:4" ht="41.25">
+      <c r="A11" s="29"/>
+      <c r="C11" s="29"/>
+    </row>
+    <row r="12" spans="1:4" ht="41.25">
+      <c r="A12" s="29"/>
+      <c r="C12" s="29"/>
+    </row>
+    <row r="13" spans="1:4" ht="41.25">
+      <c r="A13" s="29"/>
+      <c r="C13" s="29"/>
+    </row>
+    <row r="14" spans="1:4" ht="41.25">
+      <c r="A14" s="29"/>
+      <c r="C14" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="2833" scale="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4993,6 +5163,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11247,6 +11418,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12021,6 +12193,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12157,6 +12330,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -12942,6 +13116,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:L778"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -40131,7 +40306,7 @@
         <v>1076</v>
       </c>
       <c r="I771" s="17" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="J771">
         <v>7</v>
@@ -40167,7 +40342,7 @@
         <v>1077</v>
       </c>
       <c r="I772" s="17" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="J772">
         <v>8</v>
@@ -40203,7 +40378,7 @@
         <v>1078</v>
       </c>
       <c r="I773" s="17" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="J773">
         <v>9</v>
@@ -40239,7 +40414,7 @@
         <v>1079</v>
       </c>
       <c r="I774" s="17" t="s">
-        <v>1098</v>
+        <v>1122</v>
       </c>
       <c r="J774">
         <v>10</v>
@@ -40249,7 +40424,7 @@
       </c>
       <c r="L774" t="str">
         <f t="shared" si="29"/>
-        <v>insert into ms_module values('141','SOPNAME','M','','f10','text2','75','System Qty','SUM(a.beginqty+a.inqty+a.outqty)','10','TRUE');</v>
+        <v>insert into ms_module values('141','SOPNAME','M','','f10','text2','75','System Qty','SUM(a.beginqty)+SUM(a.inqty)-SUM(a.outqty) ','10','TRUE');</v>
       </c>
     </row>
     <row r="775" spans="1:12" ht="16.5" customHeight="1">
@@ -40266,7 +40441,7 @@
         <v>131</v>
       </c>
       <c r="F775" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="G775">
         <v>85</v>
@@ -40275,7 +40450,7 @@
         <v>1081</v>
       </c>
       <c r="I775" s="17" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="J775">
         <v>11</v>
@@ -40311,7 +40486,7 @@
         <v>1080</v>
       </c>
       <c r="I776" s="17" t="s">
-        <v>1094</v>
+        <v>1123</v>
       </c>
       <c r="J776">
         <v>12</v>
@@ -40321,7 +40496,7 @@
       </c>
       <c r="L776" t="str">
         <f t="shared" si="29"/>
-        <v>insert into ms_module values('143','SOPNAME','M','','f12','text2','99','Diff Qty','SUM(a.beginqty+a.inqty+a.outqty-a.opnameqty)','12','TRUE');</v>
+        <v>insert into ms_module values('143','SOPNAME','M','','f12','text2','99','Diff Qty','SUM(a.beginqty)+SUM(a.inqty)-SUM(a.outqty) -sum(a.opnameqty)','12','TRUE');</v>
       </c>
     </row>
     <row r="777" spans="1:12" ht="16.5" customHeight="1">
@@ -40341,7 +40516,7 @@
         <v>133</v>
       </c>
       <c r="I777" t="s">
-        <v>1100</v>
+        <v>1120</v>
       </c>
       <c r="J777">
         <v>13</v>
@@ -40351,7 +40526,7 @@
       </c>
       <c r="L777" t="str">
         <f t="shared" si="29"/>
-        <v>insert into ms_module values('144','SOPNAME','M','','','end','','nowhere','; from tx_stock_all a where a.itemcode&lt;&gt;"" GROUP BY a.itemname,a.warehouse,IFNULL(a.unit,"") order by itemname ;','13','TRUE');</v>
+        <v>insert into ms_module values('144','SOPNAME','M','','','end','','nowhere','; from tx_stock_all a where a.itemcode&lt;&gt;"" and transtime&gt;=(select description from ms_setting where settingtype="opnamestart") GROUP BY a.itemname,a.warehouse,IFNULL(a.unit,"") order by itemname ;','13','TRUE');</v>
       </c>
     </row>
     <row r="778" spans="1:12" ht="16.5" customHeight="1">
@@ -40371,7 +40546,7 @@
         <v>134</v>
       </c>
       <c r="I778" t="s">
-        <v>1101</v>
+        <v>1119</v>
       </c>
       <c r="J778">
         <v>14</v>
@@ -40381,7 +40556,7 @@
       </c>
       <c r="L778" t="str">
         <f t="shared" si="29"/>
-        <v>insert into ms_module values('145','SOPNAME','M','','','end','','where','; from tx_stock_all a where   a.itemcode&lt;&gt;"" and concat(itemname) like "%w2%"  GROUP BY a.itemname,a.warehouse,IFNULL(a.unit,"")  order by itemname ;','14','TRUE');</v>
+        <v>insert into ms_module values('145','SOPNAME','M','','','end','','where','; from tx_stock_all a where   a.itemcode&lt;&gt;"" and transtime&gt;=(select description from ms_setting where settingtype="opnamestart")  and concat(itemname) like "%w2%"  GROUP BY a.itemname,a.warehouse,IFNULL(a.unit,"")  order by itemname ;','14','TRUE');</v>
       </c>
     </row>
   </sheetData>
@@ -40396,9 +40571,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+    <sheetView topLeftCell="A96" workbookViewId="0">
       <selection activeCell="M96" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
@@ -41154,10 +41330,10 @@
         <v>561</v>
       </c>
       <c r="D56" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="E56" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="M56" t="str">
         <f t="shared" ref="M56:M58" si="4">"if ($q=="&amp;A56&amp;"){$query="&amp;C56&amp;D56&amp;E56&amp;F56&amp;G56&amp;H56&amp;I56&amp;J56&amp;K56&amp;L56&amp;"}"</f>
@@ -41175,13 +41351,13 @@
         <v>558</v>
       </c>
       <c r="D57" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="E57" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="F57" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="M57" t="str">
         <f t="shared" si="4"/>
@@ -41196,7 +41372,7 @@
         <v>554</v>
       </c>
       <c r="C58" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="D58" t="s">
         <v>555</v>
@@ -41274,10 +41450,10 @@
         <v>621</v>
       </c>
       <c r="D62" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="E62" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="M62" t="str">
         <f t="shared" si="5"/>
@@ -41295,13 +41471,13 @@
         <v>623</v>
       </c>
       <c r="D63" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="E63" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="F63" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="M63" t="str">
         <f t="shared" si="5"/>
@@ -41316,7 +41492,7 @@
         <v>610</v>
       </c>
       <c r="C64" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="D64" t="s">
         <v>611</v>
@@ -41394,10 +41570,10 @@
         <v>664</v>
       </c>
       <c r="D68" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="E68" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="M68" t="str">
         <f t="shared" si="5"/>
@@ -41415,13 +41591,13 @@
         <v>663</v>
       </c>
       <c r="D69" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="E69" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="F69" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="M69" t="str">
         <f t="shared" si="5"/>
@@ -41436,7 +41612,7 @@
         <v>652</v>
       </c>
       <c r="C70" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="D70" t="s">
         <v>654</v>
@@ -41520,10 +41696,10 @@
         <v>703</v>
       </c>
       <c r="D74" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="E74" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="M74" t="str">
         <f t="shared" si="6"/>
@@ -41541,13 +41717,13 @@
         <v>701</v>
       </c>
       <c r="D75" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="E75" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="F75" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="M75" t="str">
         <f t="shared" si="6"/>
@@ -41562,7 +41738,7 @@
         <v>699</v>
       </c>
       <c r="C76" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="D76" t="s">
         <v>700</v>
@@ -42089,9 +42265,12 @@
       <c r="D105" t="s">
         <v>969</v>
       </c>
+      <c r="E105" t="s">
+        <v>1121</v>
+      </c>
       <c r="M105" t="str">
         <f t="shared" si="11"/>
-        <v>if ($q=="SBupdate"){$query="delete from tx_stock_begin where txid='$dt[0]'";$str="insert into tx_stock_begin(itemcode,itemname,warehouse,qty,unit,createdate,updatedate) values('$dt[1]','$dt[2]','$dt[3]','$dt[4]','$dt[5]',now(),now())";include("exec2.php"); }</v>
+        <v>if ($q=="SBupdate"){$query="delete from tx_stock_begin where txid='$dt[0]'";$str="insert into tx_stock_begin(itemcode,itemname,warehouse,qty,unit,createdate,updatedate) values('$dt[1]','$dt[2]','$dt[3]','$dt[4]','$dt[5]',now(),now())";include("exec2.php"); $str="insert into tx_stock_all(itemcode,itemname,userid,transtime,transdesc,warehouse,inqty,outqty,beginqty,opnameqty,unit) values('$dt[1]','$dt[2]','$user',now(),'Begin Stock','$dt[3]',0,0,'$dt[4]',0,'$dt[5]')";include("exec2.php"); }</v>
       </c>
     </row>
     <row r="106" spans="1:13">
@@ -42180,7 +42359,7 @@
         <v>1053</v>
       </c>
       <c r="M110" t="str">
-        <f t="shared" ref="M110:M117" si="13">"if ($q=="&amp;A110&amp;"){$query="&amp;C110&amp;D110&amp;E110&amp;F110&amp;G110&amp;H110&amp;I110&amp;J110&amp;K110&amp;L110&amp;"}"</f>
+        <f t="shared" ref="M110:M115" si="13">"if ($q=="&amp;A110&amp;"){$query="&amp;C110&amp;D110&amp;E110&amp;F110&amp;G110&amp;H110&amp;I110&amp;J110&amp;K110&amp;L110&amp;"}"</f>
         <v>if ($q=="COTinsert"){$query="insert into tx_cash(cashno,cashdate,cashtype,bankid,totalamount,notes,createby,createdate,updateby,updatedate) values('$dt[0]','$dt[1]','COT','$dt[2]','$dt[3]','$dt[4]','$dt[5]',now(),'$dt[5]',now())";$i=0; $dt1=explode('{}', $dt[6]); if ($dt1!='') {   foreach($dt1 as $loop)   {$dt2 = explode('[]',$dt1[$i]); $str = "insert into tx_cash_d(cashno,cashid,accountcode,accountname,credit) values('$dt2[0]','$dt2[1]','$dt2[2]','$dt2[3]','$dt2[4]')"; include("exec2.php");   $i++; } }}</v>
       </c>
     </row>
@@ -42249,13 +42428,13 @@
         <v>985</v>
       </c>
       <c r="D114" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="E114" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="F114" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="M114" t="str">
         <f t="shared" si="13"/>
@@ -42270,7 +42449,7 @@
         <v>1087</v>
       </c>
       <c r="C115" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="M115" t="str">
         <f t="shared" si="13"/>
@@ -42317,6 +42496,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
report & load transaction
</commit_message>
<xml_diff>
--- a/madju-credit.xlsx
+++ b/madju-credit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6580" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6657" uniqueCount="1211">
   <si>
     <t>No</t>
   </si>
@@ -3542,6 +3542,237 @@
   </si>
   <si>
     <t>*9005*</t>
+  </si>
+  <si>
+    <t>RS01</t>
+  </si>
+  <si>
+    <t>SALES DETAIL</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,a.transid AS f1,DATE_FORMAT(transtime,'%d/%m/%Y') AS f2,rowno AS f3,c.itemid AS f4,(SELECT itemname FROM ms_item b WHERE c.itemid=b.itemcode LIMIT 1) AS f5,qty AS f6,format(itemprice,0) AS f7,format(-(discpercent/100)*itemprice,0) AS f8,format(ifnull(c.totalamount,0),0) AS f9,c.unit as f10, (SELECT format(SUM(e.totalamount),0) FROM tx_trans d LEFT JOIN tx_trans_item e ON d.transid=e.transid WHERE DATE_FORMAT(d.transtime,'%d/%m/%Y')=DATE_FORMAT(a.transtime,'%d/%m/%Y')) AS f11 FROM tx_trans a LEFT JOIN tx_trans_item c ON a.transid=c.transid WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59' GROUP BY DATE_FORMAT(transtime,'%d/%m/%Y'),itemid order by a.transid";</t>
+  </si>
+  <si>
+    <t>SALES DAILY</t>
+  </si>
+  <si>
+    <t>RS02</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,a.transid AS f1,DATE_FORMAT(transtime,'%d/%m/%Y') AS f2, IFNULL((SELECT salesname FROM ms_salesman b WHERE b.salesid=a.salesid),'')AS f3, IFNULL((SELECT membername FROM ms_membership c WHERE c.memberid=a.memberid),'') AS f4, cashierid AS f5, FORMAT(a.subtotal,0) AS f6,  a.subtotal AS i1 FROM tx_trans a WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59' ORDER BY transid";</t>
+  </si>
+  <si>
+    <t>RS03</t>
+  </si>
+  <si>
+    <t>SALES MONTHLY SALESMAN</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,DATE_FORMAT(transtime,'%d/%m/%Y') AS f1, DATE_FORMAT(transtime,'%m/%Y') AS f2, IFNULL((SELECT salesname FROM ms_salesman b WHERE b.salesid=a.salesid),'')AS f3,   format(SUM(a.subtotal),0) AS f4,(SELECT FORMAT(SUM(subtotal),0) FROM tx_trans b WHERE b.salesid=a.salesid AND DATE_FORMAT(a.transtime,'%m/%Y')=DATE_FORMAT(b.transtime,'%m/%Y') AND  b.transtime&gt;='$dt[0] 00:00' AND b.transtime&lt;='$dt[1] 23:59' ) AS f5 FROM tx_trans a WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59'  GROUP BY  DATE_FORMAT(transtime,'%d/%m/%Y'),DATE_FORMAT(transtime,'%m/%Y'),salesid ORDER BY transtime ";</t>
+  </si>
+  <si>
+    <t>SALES MONTHLY MEMBERSHIP</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,DATE_FORMAT(transtime,'%d/%m/%Y') AS f1, DATE_FORMAT(transtime,'%m/%Y') AS f2, IFNULL((SELECT membername FROM ms_membership b WHERE b.memberid=a.memberid),'') AS f3,   format(SUM(a.subtotal),0) AS f4,(SELECT FORMAT(SUM(subtotal),0) FROM tx_trans b WHERE b.memberid=a.memberid AND DATE_FORMAT(a.transtime,'%m/%Y')=DATE_FORMAT(b.transtime,'%m/%Y') AND  b.transtime&gt;='$dt[0] 00:00' AND b.transtime&lt;='$dt[1] 23:59' ) AS f5 FROM tx_trans a WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59'  GROUP BY  DATE_FORMAT(transtime,'%d/%m/%Y'),DATE_FORMAT(transtime,'%m/%Y'),memberid ORDER BY transtime ";</t>
+  </si>
+  <si>
+    <t>RS04</t>
+  </si>
+  <si>
+    <t>SALES MONTHLY CASHIER</t>
+  </si>
+  <si>
+    <t>RS05</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,DATE_FORMAT(transtime,'%d/%m/%Y') AS f1, DATE_FORMAT(transtime,'%m/%Y') AS f2, IFNULL(a.cashierid,'') AS f3,   format(SUM(a.subtotal),0) AS f4,(SELECT FORMAT(SUM(subtotal),0) FROM tx_trans b WHERE b.cashierid=a.cashierid AND DATE_FORMAT(a.transtime,'%m/%Y')=DATE_FORMAT(b.transtime,'%m/%Y') AND  b.transtime&gt;='$dt[0] 00:00' AND b.transtime&lt;='$dt[1] 23:59' ) AS f5 FROM tx_trans a WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59'  GROUP BY  DATE_FORMAT(transtime,'%d/%m/%Y'),DATE_FORMAT(transtime,'%m/%Y'),cashierid ORDER BY transtime ";</t>
+  </si>
+  <si>
+    <t>RS06</t>
+  </si>
+  <si>
+    <t>CASHIER REPORT</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,cashierid AS f1,DATE_FORMAT(transtime,'%d/%m/%y') AS f2, setorantype AS f3, description AS f4,  FORMAT(SUM(amount),0) AS F5,(SELECT FORMAT(SUM(amount),0) FROM tx_trans c LEFT JOIN tx_trans_pay d ON c.transid=d.transid  WHERE  DATE_FORMAT(a.transtime,'%d/%M/%y')=DATE_FORMAT(c.transtime,'%d/%M/%y') AND setorantype IN ('Cash','CreditCard','Debit','Transfer','Voucher')) AS f6 FROM tx_trans a LEFT JOIN tx_trans_pay b ON a.transid=b.transid  WHERE transtime&gt;='$dt[0]' AND transtime&lt;='$dt[1]'  AND setorantype IN ('Cash','CreditCard','Debit','Transfer','Voucher') GROUP BY  cashierid, DATE_FORMAT(transtime,'%d/%M/%y'), setorantype, description ORDER BY cashierid,transtime DESC, setorantype, description";</t>
+  </si>
+  <si>
+    <t>RS07</t>
+  </si>
+  <si>
+    <t>RS08</t>
+  </si>
+  <si>
+    <t>TOP SALES BY AMOUNT</t>
+  </si>
+  <si>
+    <t>TOP SALES BY QTY</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,itemid AS f1,(SELECT itemname FROM ms_item WHERE b.itemid=ms_item.itemcode LIMIT 1)AS f2, IFNULL(SUM(b.qty),0) AS f3  ,'$dt[0]' AS f4, '$dt[1]' AS f5 FROM tx_trans a LEFT JOIN tx_trans_item b ON a.transid=b.transid  WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59'  GROUP BY itemid ORDER BY SUM(b.qty) DESC LIMIT 50";</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,itemid AS f1,(SELECT itemname FROM ms_item WHERE b.itemid=ms_item.itemcode LIMIT 1)AS f2, format(SUM(b.totalamount),0) AS f3  ,'$dt[0]' AS f4, '$dt[1]' AS f5 FROM tx_trans a LEFT JOIN tx_trans_item b ON a.transid=b.transid  WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59'  GROUP BY itemid ORDER BY SUM(b.totalamount) DESC LIMIT 50";</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, suppname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dp,0) AS f22 FROM tx_purchase a  LEFT JOIN tx_purchase_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";</t>
+  </si>
+  <si>
+    <t>P001</t>
+  </si>
+  <si>
+    <t>P002</t>
+  </si>
+  <si>
+    <t>P003</t>
+  </si>
+  <si>
+    <t>P005</t>
+  </si>
+  <si>
+    <t>SALES REQUEST</t>
+  </si>
+  <si>
+    <t>PURCHASE REQUEST</t>
+  </si>
+  <si>
+    <t>PURCHASE ORDER</t>
+  </si>
+  <si>
+    <t>PURCHASE INVOICE</t>
+  </si>
+  <si>
+    <t>PURCHASE PAYMENT</t>
+  </si>
+  <si>
+    <t>Combo Report PO</t>
+  </si>
+  <si>
+    <t>Combo Report PI</t>
+  </si>
+  <si>
+    <t>Combo Report PP</t>
+  </si>
+  <si>
+    <t>"select reportid as code,reportname as name from ms_report where reportcode='PO'";</t>
+  </si>
+  <si>
+    <t>"select reportid as code,reportname as name from ms_report where reportcode='PI'";</t>
+  </si>
+  <si>
+    <t>"select reportid as code,reportname as name from ms_report where reportcode='PP'";</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, custname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dppo,0) AS f22,FORMAT(cash,0) AS f23,FORMAT(credit,0) AS f24,(SELECT setorantype FROM ms_payment d WHERE a.payterms=d.paymentid) AS f25 FROM tx_purchaseinvoice a  LEFT JOIN tx_purchaseinvoice_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.payno AS f1, a.paydate AS f2, a.custname AS f3, paymenttype  AS f4, payid AS f5, invoiceno AS f6, invdate AS f7, format(netamount,0) AS f8, format(payed,0) AS f9, format(total,0) AS f10, format(payamount,0) AS f11, format((SELECT SUM(payamount) FROM tx_purchasepay_d c WHERE b.payno=c.payno),0) AS f12,notes AS f13 FROM tx_purchasepay a LEFT JOIN tx_purchasepay_d b ON a.payno=b.payno WHERE a.payno='$dt[0]'";</t>
+  </si>
+  <si>
+    <t>C001</t>
+  </si>
+  <si>
+    <t>C002</t>
+  </si>
+  <si>
+    <t>C003</t>
+  </si>
+  <si>
+    <t>C005</t>
+  </si>
+  <si>
+    <t>KONSINYASI REQUEST</t>
+  </si>
+  <si>
+    <t>KONSINYASI ORDER</t>
+  </si>
+  <si>
+    <t>KONSINYASI INVOICE</t>
+  </si>
+  <si>
+    <t>KONSINYASI PAYMENT</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, suppname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dp,0) AS f22 FROM tx_consignment a  LEFT JOIN tx_consignment_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]'" ;</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, suppname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dp,0) AS f22 FROM tx_consignment a  LEFT JOIN tx_consignment_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, custname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dppo,0) AS f22,FORMAT(cash,0) AS f23,FORMAT(credit,0) AS f24,(SELECT setorantype FROM ms_payment d WHERE a.payterms=d.paymentid) AS f25 FROM tx_consignmentinvoice a  LEFT JOIN tx_consignmentinvoice_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]'" ;</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.payno AS f1, a.paydate AS f2, a.custname AS f3, paymenttype  AS f4, payid AS f5, invoiceno AS f6, invdate AS f7, format(netamount,0) AS f8, format(payed,0) AS f9, format(total,0) AS f10, format(payamount,0) AS f11, format((SELECT SUM(payamount) FROM tx_consignmentpay_d c WHERE b.payno=c.payno),0) AS f12,notes AS f13 FROM tx_consignmentpay a LEFT JOIN tx_consignmentpay_d b ON a.payno=b.payno WHERE a.payno='$dt[0]'";</t>
+  </si>
+  <si>
+    <t>Combo Report CO</t>
+  </si>
+  <si>
+    <t>Combo Report CI</t>
+  </si>
+  <si>
+    <t>Combo Report CP</t>
+  </si>
+  <si>
+    <t>"select reportid as code,reportname as name from ms_report where reportcode='CO'";</t>
+  </si>
+  <si>
+    <t>"select reportid as code,reportname as name from ms_report where reportcode='CI'";</t>
+  </si>
+  <si>
+    <t>"select reportid as code,reportname as name from ms_report where reportcode='CP'";</t>
+  </si>
+  <si>
+    <t>"select reportid as code,reportname as name from ms_report where reportcode='DO'";</t>
+  </si>
+  <si>
+    <t>DELIVERY ORDER</t>
+  </si>
+  <si>
+    <t>D001</t>
+  </si>
+  <si>
+    <t>Combo Report DO</t>
+  </si>
+  <si>
+    <t>Combo Report DT</t>
+  </si>
+  <si>
+    <t>Combo Report DR</t>
+  </si>
+  <si>
+    <t>"select reportid as code,reportname as name from ms_report where reportcode='DT'";</t>
+  </si>
+  <si>
+    <t>"select reportid as code,reportname as name from ms_report where reportcode='DR'";</t>
+  </si>
+  <si>
+    <t>D002</t>
+  </si>
+  <si>
+    <t>D003</t>
+  </si>
+  <si>
+    <t>DELIVERY OUT</t>
+  </si>
+  <si>
+    <t>DELIVERY RECEIVED</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, custname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, a.notes AS f13,DATE_FORMAT(deliverydate,'%d/%m/%Y') AS f14, (SELECT warehousename FROM ms_warehouse c WHERE a.warehousefrom=c.warehouseid)AS f15,(SELECT shipname FROM ms_shipping d WHERE a.shipvia=d.shipid) AS f16,deliverypic AS f17,deliveryphone AS f18,deliveryaddress AS f19 FROM tx_deliveryout a  LEFT JOIN tx_deliveryout_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, custname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, a.notes AS f13, DATE_FORMAT(deliverydate,'%d/%m/%Y') AS f14, (SELECT warehousename FROM ms_warehouse c WHERE a.warehousefrom=c.warehouseid)AS f15,(SELECT shipname FROM ms_shipping d WHERE a.shipvia=d.shipid) AS f16,deliverypic AS f17,deliveryphone AS f18,deliveryaddress AS f19 FROM tx_delivery a  LEFT JOIN tx_delivery_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";</t>
+  </si>
+  <si>
+    <t>"SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, custname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, a.notes AS f13,DATE_FORMAT(deliverydate,'%d/%m/%Y') AS f14, (SELECT warehousename FROM ms_warehouse c WHERE a.warehousefrom=c.warehouseid)AS f15,(SELECT shipname FROM ms_shipping d WHERE a.shipvia=d.shipid) AS f16,deliverypic AS f17,deliveryphone AS f18,deliveryaddress AS f19 FROM tx_deliveryreceived a  LEFT JOIN tx_deliveryreceived_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";</t>
+  </si>
+  <si>
+    <t>Sales Order Query</t>
+  </si>
+  <si>
+    <t>"SELECT orderno AS f1, orderdate AS f2,transtype AS f3, custcode AS f4, custname AS f5, (SELECT setorantype FROM ms_payment WHERE paymentid=tx_sales.payterms LIMIT 1) AS f6, refno AS f7, (SELECT salesname FROM ms_salesman WHERE salesid=tx_sales.salesman LIMIT 1) AS f8, totalamount AS f9, discent AS f10, disamount AS f11, ppncent AS f12, otherfee AS f13, FORMAT(netamount,0) AS f14, shipvia AS f15, deliveryto AS f16, deliveryaddress AS f17, deliverypic AS f18, deliveryphone AS f19, deliverydate AS f20, (SELECT warehousename FROM ms_warehouse WHERE warehouseid=tx_sales.warehousefrom LIMIT 1) AS f21, field1 AS f22, field2 AS f23, field3 AS f24, field4 AS f25, field5 AS f26, field6 AS f27, invtaxno1 AS f28,invtaxno2 AS f29, invtaxdate AS f30, invtaxmemo AS f31,notes AS f32,(SELECT GROUP_CONCAT(c.orderid,'[',c.prodcode,'[',c.prodname,'[',c.qty,'[',c.unit,'[',c.price,'[',c.discent,'[',c.disamount,'[',c.total SEPARATOR '{')FROM tx_sales_d c WHERE tx_sales.orderno=c.orderno) AS f33, dp AS f34,leftamount AS f35,ppnamount AS f36 FROM tx_sales  WHERE orderno='$dt[0]'";</t>
   </si>
 </sst>
 </file>
@@ -3636,7 +3867,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
@@ -3704,6 +3935,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4769,16 +5003,16 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -4827,7 +5061,7 @@
         <v>993</v>
       </c>
       <c r="B2" t="s">
-        <v>1018</v>
+        <v>1163</v>
       </c>
       <c r="C2" t="s">
         <v>1020</v>
@@ -4897,8 +5131,293 @@
         <v>if ($q=='S005'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.payno AS f1, a.paydate AS f2, a.custname AS f3, paymenttype  AS f4, payid AS f5, invoiceno AS f6, invdate AS f7, format(netamount,0) AS f8, format(payed,0) AS f9, format(total,0) AS f10, format(payamount,0) AS f11, format((SELECT SUM(payamount) FROM tx_salespay_d c WHERE b.payno=c.payno),0) AS f12,notes AS f13 FROM tx_salespay a LEFT JOIN tx_salespay_d b ON a.payno=b.payno WHERE a.payno='$dt[0]'";}</v>
       </c>
     </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1158</v>
+      </c>
+      <c r="M7" t="str">
+        <f>"if ($q=='"&amp;A7&amp;"'){$query="&amp;C7&amp;D7&amp;E7&amp;F7&amp;G7&amp;H7&amp;I7&amp;J7&amp;K7&amp;L7&amp;"}"</f>
+        <v>if ($q=='P001'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, suppname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dp,0) AS f22 FROM tx_purchase a  LEFT JOIN tx_purchase_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1158</v>
+      </c>
+      <c r="M8" t="str">
+        <f>"if ($q=='"&amp;A8&amp;"'){$query="&amp;C8&amp;D8&amp;E8&amp;F8&amp;G8&amp;H8&amp;I8&amp;J8&amp;K8&amp;L8&amp;"}"</f>
+        <v>if ($q=='P002'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, suppname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dp,0) AS f22 FROM tx_purchase a  LEFT JOIN tx_purchase_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1174</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" ref="M9:M10" si="0">"if ($q=='"&amp;A9&amp;"'){$query="&amp;C9&amp;D9&amp;E9&amp;F9&amp;G9&amp;H9&amp;I9&amp;J9&amp;K9&amp;L9&amp;"}"</f>
+        <v>if ($q=='P003'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, custname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dppo,0) AS f22,FORMAT(cash,0) AS f23,FORMAT(credit,0) AS f24,(SELECT setorantype FROM ms_payment d WHERE a.payterms=d.paymentid) AS f25 FROM tx_purchaseinvoice a  LEFT JOIN tx_purchaseinvoice_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1175</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>if ($q=='P005'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.payno AS f1, a.paydate AS f2, a.custname AS f3, paymenttype  AS f4, payid AS f5, invoiceno AS f6, invdate AS f7, format(netamount,0) AS f8, format(payed,0) AS f9, format(total,0) AS f10, format(payamount,0) AS f11, format((SELECT SUM(payamount) FROM tx_purchasepay_d c WHERE b.payno=c.payno),0) AS f12,notes AS f13 FROM tx_purchasepay a LEFT JOIN tx_purchasepay_d b ON a.payno=b.payno WHERE a.payno='$dt[0]'";}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>1184</v>
+      </c>
+      <c r="M11" t="str">
+        <f>"if ($q=='"&amp;A11&amp;"'){$query="&amp;C11&amp;D11&amp;E11&amp;F11&amp;G11&amp;H11&amp;I11&amp;J11&amp;K11&amp;L11&amp;"}"</f>
+        <v>if ($q=='C001'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, suppname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dp,0) AS f22 FROM tx_consignment a  LEFT JOIN tx_consignment_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]'" ;}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>1185</v>
+      </c>
+      <c r="M12" t="str">
+        <f>"if ($q=='"&amp;A12&amp;"'){$query="&amp;C12&amp;D12&amp;E12&amp;F12&amp;G12&amp;H12&amp;I12&amp;J12&amp;K12&amp;L12&amp;"}"</f>
+        <v>if ($q=='C002'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, suppname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dp,0) AS f22 FROM tx_consignment a  LEFT JOIN tx_consignment_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>1186</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" ref="M13:M14" si="1">"if ($q=='"&amp;A13&amp;"'){$query="&amp;C13&amp;D13&amp;E13&amp;F13&amp;G13&amp;H13&amp;I13&amp;J13&amp;K13&amp;L13&amp;"}"</f>
+        <v>if ($q=='C003'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, custname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, FORMAT(price,0) AS f10, b.discent AS f11, FORMAT(total,0) AS f12, a.notes AS f13, FORMAT(totalamount,0) AS f15, a.discent AS f16, FORMAT(a.disamount,0) AS f17, ppncent AS f18, FORMAT(ppnamount,0) AS f19, FORMAT(otherfee,0) AS f20, FORMAT(netamount,0) AS f21, FORMAT(dppo,0) AS f22,FORMAT(cash,0) AS f23,FORMAT(credit,0) AS f24,(SELECT setorantype FROM ms_payment d WHERE a.payterms=d.paymentid) AS f25 FROM tx_consignmentinvoice a  LEFT JOIN tx_consignmentinvoice_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]'" ;}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>1187</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>if ($q=='C005'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.payno AS f1, a.paydate AS f2, a.custname AS f3, paymenttype  AS f4, payid AS f5, invoiceno AS f6, invdate AS f7, format(netamount,0) AS f8, format(payed,0) AS f9, format(total,0) AS f10, format(payamount,0) AS f11, format((SELECT SUM(payamount) FROM tx_consignmentpay_d c WHERE b.payno=c.payno),0) AS f12,notes AS f13 FROM tx_consignmentpay a LEFT JOIN tx_consignmentpay_d b ON a.payno=b.payno WHERE a.payno='$dt[0]'";}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="M15" t="str">
+        <f>"if ($q=='"&amp;A15&amp;"'){$query="&amp;C15&amp;D15&amp;E15&amp;F15&amp;G15&amp;H15&amp;I15&amp;J15&amp;K15&amp;L15&amp;"}"</f>
+        <v>if ($q=='D001'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, custname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, a.notes AS f13, DATE_FORMAT(deliverydate,'%d/%m/%Y') AS f14, (SELECT warehousename FROM ms_warehouse c WHERE a.warehousefrom=c.warehouseid)AS f15,(SELECT shipname FROM ms_shipping d WHERE a.shipvia=d.shipid) AS f16,deliverypic AS f17,deliveryphone AS f18,deliveryaddress AS f19 FROM tx_delivery a  LEFT JOIN tx_delivery_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";}</v>
+      </c>
+    </row>
     <row r="16" spans="1:13">
-      <c r="M16" t="s">
+      <c r="A16" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1206</v>
+      </c>
+      <c r="M16" t="str">
+        <f>"if ($q=='"&amp;A16&amp;"'){$query="&amp;C16&amp;D16&amp;E16&amp;F16&amp;G16&amp;H16&amp;I16&amp;J16&amp;K16&amp;L16&amp;"}"</f>
+        <v>if ($q=='D002'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, custname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, a.notes AS f13,DATE_FORMAT(deliverydate,'%d/%m/%Y') AS f14, (SELECT warehousename FROM ms_warehouse c WHERE a.warehousefrom=c.warehouseid)AS f15,(SELECT shipname FROM ms_shipping d WHERE a.shipvia=d.shipid) AS f16,deliverypic AS f17,deliveryphone AS f18,deliveryaddress AS f19 FROM tx_deliveryout a  LEFT JOIN tx_deliveryout_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1208</v>
+      </c>
+      <c r="M17" t="str">
+        <f>"if ($q=='"&amp;A17&amp;"'){$query="&amp;C17&amp;D17&amp;E17&amp;F17&amp;G17&amp;H17&amp;I17&amp;J17&amp;K17&amp;L17&amp;"}"</f>
+        <v>if ($q=='D003'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5, a.orderno AS f1, orderdate AS f2, custname AS f3,  IFNULL((SELECT salesname FROM ms_salesman c WHERE a.salesman=c.salesid),'') AS f4, orderid AS f5, prodcode AS f6, prodname AS f7, qty AS f8, unit AS f9, a.notes AS f13,DATE_FORMAT(deliverydate,'%d/%m/%Y') AS f14, (SELECT warehousename FROM ms_warehouse c WHERE a.warehousefrom=c.warehouseid)AS f15,(SELECT shipname FROM ms_shipping d WHERE a.shipvia=d.shipid) AS f16,deliverypic AS f17,deliveryphone AS f18,deliveryaddress AS f19 FROM tx_deliveryreceived a  LEFT JOIN tx_deliveryreceived_d b  ON a.orderno=b.orderno WHERE a.orderno='$dt[0]' ";}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1136</v>
+      </c>
+      <c r="M18" t="str">
+        <f>"if ($q=='"&amp;A18&amp;"'){$query="&amp;C18&amp;D18&amp;E18&amp;F18&amp;G18&amp;H18&amp;I18&amp;J18&amp;K18&amp;L18&amp;"}"</f>
+        <v>if ($q=='RS01'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,a.transid AS f1,DATE_FORMAT(transtime,'%d/%m/%Y') AS f2,rowno AS f3,c.itemid AS f4,(SELECT itemname FROM ms_item b WHERE c.itemid=b.itemcode LIMIT 1) AS f5,qty AS f6,format(itemprice,0) AS f7,format(-(discpercent/100)*itemprice,0) AS f8,format(ifnull(c.totalamount,0),0) AS f9,c.unit as f10, (SELECT format(SUM(e.totalamount),0) FROM tx_trans d LEFT JOIN tx_trans_item e ON d.transid=e.transid WHERE DATE_FORMAT(d.transtime,'%d/%m/%Y')=DATE_FORMAT(a.transtime,'%d/%m/%Y')) AS f11 FROM tx_trans a LEFT JOIN tx_trans_item c ON a.transid=c.transid WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59' GROUP BY DATE_FORMAT(transtime,'%d/%m/%Y'),itemid order by a.transid";}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>1139</v>
+      </c>
+      <c r="M19" t="str">
+        <f>"if ($q=='"&amp;A19&amp;"'){$query="&amp;C19&amp;D19&amp;E19&amp;F19&amp;G19&amp;H19&amp;I19&amp;J19&amp;K19&amp;L19&amp;"}"</f>
+        <v>if ($q=='RS02'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,a.transid AS f1,DATE_FORMAT(transtime,'%d/%m/%Y') AS f2, IFNULL((SELECT salesname FROM ms_salesman b WHERE b.salesid=a.salesid),'')AS f3, IFNULL((SELECT membername FROM ms_membership c WHERE c.memberid=a.memberid),'') AS f4, cashierid AS f5, FORMAT(a.subtotal,0) AS f6,  a.subtotal AS i1 FROM tx_trans a WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59' ORDER BY transid";}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>1142</v>
+      </c>
+      <c r="M20" t="str">
+        <f>"if ($q=='"&amp;A20&amp;"'){$query="&amp;C20&amp;D20&amp;E20&amp;F20&amp;G20&amp;H20&amp;I20&amp;J20&amp;K20&amp;L20&amp;"}"</f>
+        <v>if ($q=='RS03'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,DATE_FORMAT(transtime,'%d/%m/%Y') AS f1, DATE_FORMAT(transtime,'%m/%Y') AS f2, IFNULL((SELECT salesname FROM ms_salesman b WHERE b.salesid=a.salesid),'')AS f3,   format(SUM(a.subtotal),0) AS f4,(SELECT FORMAT(SUM(subtotal),0) FROM tx_trans b WHERE b.salesid=a.salesid AND DATE_FORMAT(a.transtime,'%m/%Y')=DATE_FORMAT(b.transtime,'%m/%Y') AND  b.transtime&gt;='$dt[0] 00:00' AND b.transtime&lt;='$dt[1] 23:59' ) AS f5 FROM tx_trans a WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59'  GROUP BY  DATE_FORMAT(transtime,'%d/%m/%Y'),DATE_FORMAT(transtime,'%m/%Y'),salesid ORDER BY transtime ";}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>1144</v>
+      </c>
+      <c r="M21" t="str">
+        <f>"if ($q=='"&amp;A21&amp;"'){$query="&amp;C21&amp;D21&amp;E21&amp;F21&amp;G21&amp;H21&amp;I21&amp;J21&amp;K21&amp;L21&amp;"}"</f>
+        <v>if ($q=='RS04'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,DATE_FORMAT(transtime,'%d/%m/%Y') AS f1, DATE_FORMAT(transtime,'%m/%Y') AS f2, IFNULL((SELECT membername FROM ms_membership b WHERE b.memberid=a.memberid),'') AS f3,   format(SUM(a.subtotal),0) AS f4,(SELECT FORMAT(SUM(subtotal),0) FROM tx_trans b WHERE b.memberid=a.memberid AND DATE_FORMAT(a.transtime,'%m/%Y')=DATE_FORMAT(b.transtime,'%m/%Y') AND  b.transtime&gt;='$dt[0] 00:00' AND b.transtime&lt;='$dt[1] 23:59' ) AS f5 FROM tx_trans a WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59'  GROUP BY  DATE_FORMAT(transtime,'%d/%m/%Y'),DATE_FORMAT(transtime,'%m/%Y'),memberid ORDER BY transtime ";}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>1148</v>
+      </c>
+      <c r="M22" t="str">
+        <f>"if ($q=='"&amp;A22&amp;"'){$query="&amp;C22&amp;D22&amp;E22&amp;F22&amp;G22&amp;H22&amp;I22&amp;J22&amp;K22&amp;L22&amp;"}"</f>
+        <v>if ($q=='RS05'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,DATE_FORMAT(transtime,'%d/%m/%Y') AS f1, DATE_FORMAT(transtime,'%m/%Y') AS f2, IFNULL(a.cashierid,'') AS f3,   format(SUM(a.subtotal),0) AS f4,(SELECT FORMAT(SUM(subtotal),0) FROM tx_trans b WHERE b.cashierid=a.cashierid AND DATE_FORMAT(a.transtime,'%m/%Y')=DATE_FORMAT(b.transtime,'%m/%Y') AND  b.transtime&gt;='$dt[0] 00:00' AND b.transtime&lt;='$dt[1] 23:59' ) AS f5 FROM tx_trans a WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59'  GROUP BY  DATE_FORMAT(transtime,'%d/%m/%Y'),DATE_FORMAT(transtime,'%m/%Y'),cashierid ORDER BY transtime ";}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>1151</v>
+      </c>
+      <c r="M23" t="str">
+        <f>"if ($q=='"&amp;A23&amp;"'){$query="&amp;C23&amp;D23&amp;E23&amp;F23&amp;G23&amp;H23&amp;I23&amp;J23&amp;K23&amp;L23&amp;"}"</f>
+        <v>if ($q=='RS06'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,cashierid AS f1,DATE_FORMAT(transtime,'%d/%m/%y') AS f2, setorantype AS f3, description AS f4,  FORMAT(SUM(amount),0) AS F5,(SELECT FORMAT(SUM(amount),0) FROM tx_trans c LEFT JOIN tx_trans_pay d ON c.transid=d.transid  WHERE  DATE_FORMAT(a.transtime,'%d/%M/%y')=DATE_FORMAT(c.transtime,'%d/%M/%y') AND setorantype IN ('Cash','CreditCard','Debit','Transfer','Voucher')) AS f6 FROM tx_trans a LEFT JOIN tx_trans_pay b ON a.transid=b.transid  WHERE transtime&gt;='$dt[0]' AND transtime&lt;='$dt[1]'  AND setorantype IN ('Cash','CreditCard','Debit','Transfer','Voucher') GROUP BY  cashierid, DATE_FORMAT(transtime,'%d/%M/%y'), setorantype, description ORDER BY cashierid,transtime DESC, setorantype, description";}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>1157</v>
+      </c>
+      <c r="M24" t="str">
+        <f>"if ($q=='"&amp;A24&amp;"'){$query="&amp;C24&amp;D24&amp;E24&amp;F24&amp;G24&amp;H24&amp;I24&amp;J24&amp;K24&amp;L24&amp;"}"</f>
+        <v>if ($q=='RS07'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,itemid AS f1,(SELECT itemname FROM ms_item WHERE b.itemid=ms_item.itemcode LIMIT 1)AS f2, format(SUM(b.totalamount),0) AS f3  ,'$dt[0]' AS f4, '$dt[1]' AS f5 FROM tx_trans a LEFT JOIN tx_trans_item b ON a.transid=b.transid  WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59'  GROUP BY itemid ORDER BY SUM(b.totalamount) DESC LIMIT 50";}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>1156</v>
+      </c>
+      <c r="M25" t="str">
+        <f>"if ($q=='"&amp;A25&amp;"'){$query="&amp;C25&amp;D25&amp;E25&amp;F25&amp;G25&amp;H25&amp;I25&amp;J25&amp;K25&amp;L25&amp;"}"</f>
+        <v>if ($q=='RS08'){$query="SELECT (SELECT companyname FROM ms_company) AS a1, (SELECT address FROM ms_company) AS a2, (SELECT phone FROM ms_company) AS a3, (SELECT fax FROM ms_company) AS a4, '$user' AS a5,itemid AS f1,(SELECT itemname FROM ms_item WHERE b.itemid=ms_item.itemcode LIMIT 1)AS f2, IFNULL(SUM(b.qty),0) AS f3  ,'$dt[0]' AS f4, '$dt[1]' AS f5 FROM tx_trans a LEFT JOIN tx_trans_item b ON a.transid=b.transid  WHERE transtime&gt;='$dt[0] 00:00' AND transtime&lt;='$dt[1] 23:59'  GROUP BY itemid ORDER BY SUM(b.qty) DESC LIMIT 50";}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="M27" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4912,7 +5431,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -12331,10 +12850,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12956,7 +13475,7 @@
         <v>913</v>
       </c>
       <c r="M39" t="str">
-        <f t="shared" ref="M39:M48" si="3">"if ($q=="&amp;A39&amp;"){$query="&amp;C39&amp;D39&amp;E39&amp;F39&amp;G39&amp;H39&amp;I39&amp;J39&amp;K39&amp;L39&amp;"}"</f>
+        <f>"if ($q=="&amp;A39&amp;"){$query="&amp;C39&amp;D39&amp;E39&amp;F39&amp;G39&amp;H39&amp;I39&amp;J39&amp;K39&amp;L39&amp;"}"</f>
         <v>if ($q==55){$query="SELECT settingid AS CODE, REPLACE(REPLACE(REPLACE(REPLACE(REPLACE(REPLACE(description,'%y',DATE_FORMAT(NOW(),'%y')),'%d',DATE_FORMAT(NOW(),'%d')),'%m',DATE_FORMAT(NOW(),'%m')),'%c5',(SELECT RIGHT(100000+IFNULL(MAX(RIGHT(orderno,5)),'100000')+1,5) FROM tx_deliveryout WHERE transtype='DT' AND DATE_FORMAT(orderdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m')))  ,'%c4',(SELECT RIGHT(10000+IFNULL(MAX(RIGHT(orderno,4)),'10000')+1,4) FROM tx_deliveryout WHERE transtype='DT' AND DATE_FORMAT(orderdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m'))),'%c3',(SELECT RIGHT(1000+IFNULL(MAX(RIGHT(orderno,3)),'1000')+1,3) FROM tx_deliveryout WHERE transtype='DT' AND  DATE_FORMAT(orderdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m'))) AS NAME FROM ms_setting WHERE settingtype='dt' ";}</v>
       </c>
     </row>
@@ -12971,7 +13490,7 @@
         <v>915</v>
       </c>
       <c r="M40" t="str">
-        <f t="shared" si="3"/>
+        <f>"if ($q=="&amp;A40&amp;"){$query="&amp;C40&amp;D40&amp;E40&amp;F40&amp;G40&amp;H40&amp;I40&amp;J40&amp;K40&amp;L40&amp;"}"</f>
         <v>if ($q==56){$query="SELECT orderno AS CODE,orderno AS NAME FROM tx_delivery ORDER BY orderno DESC LIMIT 100";}</v>
       </c>
     </row>
@@ -12986,7 +13505,7 @@
         <v>933</v>
       </c>
       <c r="M41" t="str">
-        <f t="shared" si="3"/>
+        <f>"if ($q=="&amp;A41&amp;"){$query="&amp;C41&amp;D41&amp;E41&amp;F41&amp;G41&amp;H41&amp;I41&amp;J41&amp;K41&amp;L41&amp;"}"</f>
         <v>if ($q==57){$query="SELECT settingid AS CODE, REPLACE(REPLACE(REPLACE(REPLACE(REPLACE(REPLACE(description,'%y',DATE_FORMAT(NOW(),'%y')),'%d',DATE_FORMAT(NOW(),'%d')),'%m',DATE_FORMAT(NOW(),'%m')),'%c5',(SELECT RIGHT(100000+IFNULL(MAX(RIGHT(orderno,5)),'100000')+1,5) FROM tx_deliveryreceived WHERE transtype='DR' AND DATE_FORMAT(orderdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m')))  ,'%c4',(SELECT RIGHT(10000+IFNULL(MAX(RIGHT(orderno,4)),'10000')+1,4) FROM tx_deliveryreceived WHERE transtype='DR' AND DATE_FORMAT(orderdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m'))),'%c3',(SELECT RIGHT(1000+IFNULL(MAX(RIGHT(orderno,3)),'1000')+1,3) FROM tx_deliveryreceived WHERE transtype='DR' AND  DATE_FORMAT(orderdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m'))) AS NAME FROM ms_setting WHERE settingtype='dr' ";}</v>
       </c>
     </row>
@@ -13001,7 +13520,7 @@
         <v>934</v>
       </c>
       <c r="M42" t="str">
-        <f t="shared" si="3"/>
+        <f>"if ($q=="&amp;A42&amp;"){$query="&amp;C42&amp;D42&amp;E42&amp;F42&amp;G42&amp;H42&amp;I42&amp;J42&amp;K42&amp;L42&amp;"}"</f>
         <v>if ($q==58){$query="SELECT orderno AS CODE,orderno AS NAME FROM tx_deliveryout ORDER BY orderno DESC LIMIT 100";}</v>
       </c>
     </row>
@@ -13016,7 +13535,7 @@
         <v>1019</v>
       </c>
       <c r="M43" t="str">
-        <f t="shared" si="3"/>
+        <f>"if ($q=="&amp;A43&amp;"){$query="&amp;C43&amp;D43&amp;E43&amp;F43&amp;G43&amp;H43&amp;I43&amp;J43&amp;K43&amp;L43&amp;"}"</f>
         <v>if ($q==60){$query="select reportid as code,reportname as name from ms_report where reportcode='SO'";}</v>
       </c>
     </row>
@@ -13031,7 +13550,7 @@
         <v>1023</v>
       </c>
       <c r="M44" t="str">
-        <f t="shared" si="3"/>
+        <f>"if ($q=="&amp;A44&amp;"){$query="&amp;C44&amp;D44&amp;E44&amp;F44&amp;G44&amp;H44&amp;I44&amp;J44&amp;K44&amp;L44&amp;"}"</f>
         <v>if ($q==61){$query="select reportid as code,reportname as name from ms_report where reportcode='SI'";}</v>
       </c>
     </row>
@@ -13046,7 +13565,7 @@
         <v>1028</v>
       </c>
       <c r="M45" t="str">
-        <f t="shared" si="3"/>
+        <f>"if ($q=="&amp;A45&amp;"){$query="&amp;C45&amp;D45&amp;E45&amp;F45&amp;G45&amp;H45&amp;I45&amp;J45&amp;K45&amp;L45&amp;"}"</f>
         <v>if ($q==62){$query="select reportid as code,reportname as name from ms_report where reportcode='SP'";}</v>
       </c>
     </row>
@@ -13061,7 +13580,7 @@
         <v>1035</v>
       </c>
       <c r="M46" t="str">
-        <f t="shared" si="3"/>
+        <f>"if ($q=="&amp;A46&amp;"){$query="&amp;C46&amp;D46&amp;E46&amp;F46&amp;G46&amp;H46&amp;I46&amp;J46&amp;K46&amp;L46&amp;"}"</f>
         <v>if ($q==63){$query="SELECT settingid AS CODE, REPLACE(REPLACE(REPLACE(REPLACE(REPLACE(REPLACE(description,'%y',DATE_FORMAT(NOW(),'%y')),'%d',DATE_FORMAT(NOW(),'%d')),'%m',DATE_FORMAT(NOW(),'%m')),'%c5',(SELECT RIGHT(100000+IFNULL(MAX(RIGHT(cashno,5)),'100000')+1,5) FROM tx_cash WHERE DATE_FORMAT(cashdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m')))  ,'%c4',(SELECT RIGHT(10000+IFNULL(MAX(RIGHT(cashno,4)),'10000')+1,4) FROM tx_cash WHERE DATE_FORMAT(cashdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m'))),'%c3',(SELECT RIGHT(1000+IFNULL(MAX(RIGHT(cashno,3)),'1000')+1,3) FROM tx_cash WHERE   DATE_FORMAT(cashdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m'))) AS NAME FROM ms_setting WHERE settingtype='cin' ";}</v>
       </c>
     </row>
@@ -13076,7 +13595,7 @@
         <v>1036</v>
       </c>
       <c r="M47" t="str">
-        <f t="shared" si="3"/>
+        <f>"if ($q=="&amp;A47&amp;"){$query="&amp;C47&amp;D47&amp;E47&amp;F47&amp;G47&amp;H47&amp;I47&amp;J47&amp;K47&amp;L47&amp;"}"</f>
         <v>if ($q==64){$query="SELECT settingid AS CODE, REPLACE(REPLACE(REPLACE(REPLACE(REPLACE(REPLACE(description,'%y',DATE_FORMAT(NOW(),'%y')),'%d',DATE_FORMAT(NOW(),'%d')),'%m',DATE_FORMAT(NOW(),'%m')),'%c5',(SELECT RIGHT(100000+IFNULL(MAX(RIGHT(cashno,5)),'100000')+1,5) FROM tx_cash WHERE DATE_FORMAT(cashdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m')))  ,'%c4',(SELECT RIGHT(10000+IFNULL(MAX(RIGHT(cashno,4)),'10000')+1,4) FROM tx_cash WHERE DATE_FORMAT(cashdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m'))),'%c3',(SELECT RIGHT(1000+IFNULL(MAX(RIGHT(cashno,3)),'1000')+1,3) FROM tx_cash WHERE   DATE_FORMAT(cashdate,'%y%m')=DATE_FORMAT(NOW(),'%y%m'))) AS NAME FROM ms_setting WHERE settingtype='cot' ";}</v>
       </c>
     </row>
@@ -13094,17 +13613,165 @@
         <v>1034</v>
       </c>
       <c r="M48" t="str">
+        <f>"if ($q=="&amp;A48&amp;"){$query="&amp;C48&amp;D48&amp;E48&amp;F48&amp;G48&amp;H48&amp;I48&amp;J48&amp;K48&amp;L48&amp;"}"</f>
+        <v>if ($q==65){$query="SELECT accountcode as f1,accountname as f2 FROM ms_account LIMIT 200";if ($q2!=""){$query="SELECT accountcode as f1,accountname as f2 FROM ms_account where  concat(accountcode,accountname)  like '%$dt[0]%' ORDER BY accountname  limit 200";}}</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="17.25" customHeight="1">
+      <c r="A49">
+        <v>70</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>1171</v>
+      </c>
+      <c r="M49" t="str">
+        <f>"if ($q=="&amp;A49&amp;"){$query="&amp;C49&amp;D49&amp;E49&amp;F49&amp;G49&amp;H49&amp;I49&amp;J49&amp;K49&amp;L49&amp;"}"</f>
+        <v>if ($q==70){$query="select reportid as code,reportname as name from ms_report where reportcode='PO'";}</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50">
+        <v>71</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>1172</v>
+      </c>
+      <c r="M50" t="str">
+        <f>"if ($q=="&amp;A50&amp;"){$query="&amp;C50&amp;D50&amp;E50&amp;F50&amp;G50&amp;H50&amp;I50&amp;J50&amp;K50&amp;L50&amp;"}"</f>
+        <v>if ($q==71){$query="select reportid as code,reportname as name from ms_report where reportcode='PI'";}</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51">
+        <v>72</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>1173</v>
+      </c>
+      <c r="M51" t="str">
+        <f>"if ($q=="&amp;A51&amp;"){$query="&amp;C51&amp;D51&amp;E51&amp;F51&amp;G51&amp;H51&amp;I51&amp;J51&amp;K51&amp;L51&amp;"}"</f>
+        <v>if ($q==72){$query="select reportid as code,reportname as name from ms_report where reportcode='PP'";}</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52">
+        <v>80</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>1191</v>
+      </c>
+      <c r="M52" t="str">
+        <f t="shared" ref="M52:M58" si="3">"if ($q=="&amp;A52&amp;"){$query="&amp;C52&amp;D52&amp;E52&amp;F52&amp;G52&amp;H52&amp;I52&amp;J52&amp;K52&amp;L52&amp;"}"</f>
+        <v>if ($q==80){$query="select reportid as code,reportname as name from ms_report where reportcode='CO'";}</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53">
+        <v>81</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>1192</v>
+      </c>
+      <c r="M53" t="str">
         <f t="shared" si="3"/>
-        <v>if ($q==65){$query="SELECT accountcode as f1,accountname as f2 FROM ms_account LIMIT 200";if ($q2!=""){$query="SELECT accountcode as f1,accountname as f2 FROM ms_account where  concat(accountcode,accountname)  like '%$dt[0]%' ORDER BY accountname  limit 200";}}</v>
-      </c>
-    </row>
-    <row r="49" spans="3:13" ht="17.25" customHeight="1">
-      <c r="C49" s="24" t="s">
+        <v>if ($q==81){$query="select reportid as code,reportname as name from ms_report where reportcode='CI'";}</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54">
+        <v>82</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>1193</v>
+      </c>
+      <c r="M54" t="str">
+        <f t="shared" si="3"/>
+        <v>if ($q==82){$query="select reportid as code,reportname as name from ms_report where reportcode='CP'";}</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55">
+        <v>90</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>1194</v>
+      </c>
+      <c r="M55" t="str">
+        <f t="shared" si="3"/>
+        <v>if ($q==90){$query="select reportid as code,reportname as name from ms_report where reportcode='DO'";}</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56">
+        <v>91</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>1200</v>
+      </c>
+      <c r="M56" t="str">
+        <f t="shared" si="3"/>
+        <v>if ($q==91){$query="select reportid as code,reportname as name from ms_report where reportcode='DT'";}</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57">
+        <v>92</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>1201</v>
+      </c>
+      <c r="M57" t="str">
+        <f t="shared" si="3"/>
+        <v>if ($q==92){$query="select reportid as code,reportname as name from ms_report where reportcode='DR'";}</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="20.25" customHeight="1">
+      <c r="A58">
+        <v>100</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>1210</v>
+      </c>
+      <c r="M58" t="str">
+        <f t="shared" si="3"/>
+        <v>if ($q==100){$query="SELECT orderno AS f1, orderdate AS f2,transtype AS f3, custcode AS f4, custname AS f5, (SELECT setorantype FROM ms_payment WHERE paymentid=tx_sales.payterms LIMIT 1) AS f6, refno AS f7, (SELECT salesname FROM ms_salesman WHERE salesid=tx_sales.salesman LIMIT 1) AS f8, totalamount AS f9, discent AS f10, disamount AS f11, ppncent AS f12, otherfee AS f13, FORMAT(netamount,0) AS f14, shipvia AS f15, deliveryto AS f16, deliveryaddress AS f17, deliverypic AS f18, deliveryphone AS f19, deliverydate AS f20, (SELECT warehousename FROM ms_warehouse WHERE warehouseid=tx_sales.warehousefrom LIMIT 1) AS f21, field1 AS f22, field2 AS f23, field3 AS f24, field4 AS f25, field5 AS f26, field6 AS f27, invtaxno1 AS f28,invtaxno2 AS f29, invtaxdate AS f30, invtaxmemo AS f31,notes AS f32,(SELECT GROUP_CONCAT(c.orderid,'[',c.prodcode,'[',c.prodname,'[',c.qty,'[',c.unit,'[',c.price,'[',c.discent,'[',c.disamount,'[',c.total SEPARATOR '{')FROM tx_sales_d c WHERE tx_sales.orderno=c.orderno) AS f33, dp AS f34,leftamount AS f35,ppnamount AS f36 FROM tx_sales  WHERE orderno='$dt[0]'";}</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="20.25" customHeight="1">
+      <c r="C59" s="24" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="52" spans="3:13">
-      <c r="M52" t="s">
+      <c r="M59" t="s">
         <v>98</v>
       </c>
     </row>
@@ -13120,8 +13787,8 @@
   <dimension ref="A1:L778"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A764" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I72" sqref="I71:I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
@@ -40575,7 +41242,7 @@
   <dimension ref="A1:M120"/>
   <sheetViews>
     <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="M96" sqref="M1:M1048576"/>
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>